<commit_message>
mail setup done, deployment left
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -445,7 +445,7 @@
         <v>Not Found</v>
       </c>
       <c r="E2" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F2" t="str">
         <v>3</v>
@@ -457,7 +457,7 @@
         <v>1667</v>
       </c>
       <c r="I2" t="str">
-        <v>"Good shape and great east location"</v>
+        <v>"Good shape and great east location."</v>
       </c>
     </row>
     <row r="3">
@@ -474,7 +474,7 @@
         <v>Not Found</v>
       </c>
       <c r="E3" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F3" t="str">
         <v>4</v>
@@ -486,7 +486,10 @@
         <v>1358</v>
       </c>
       <c r="I3" t="str">
-        <v>"Large lot. The property needs work"</v>
+        <v>"Large lot</v>
+      </c>
+      <c r="J3" t="str">
+        <v xml:space="preserve"> Needs work"</v>
       </c>
     </row>
     <row r="4">
@@ -503,7 +506,7 @@
         <v>Not Found</v>
       </c>
       <c r="E4" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F4" t="str">
         <v>2</v>
@@ -515,10 +518,19 @@
         <v>1092</v>
       </c>
       <c r="I4" t="str">
-        <v>"A/C 2021. New garage door. Roof 2004. New exterior paint. In good shape</v>
+        <v>"A/C 2021</v>
       </c>
       <c r="J4" t="str">
-        <v xml:space="preserve"> just needs updating"</v>
+        <v xml:space="preserve"> New garage door</v>
+      </c>
+      <c r="K4" t="str">
+        <v xml:space="preserve"> Roof 2004</v>
+      </c>
+      <c r="L4" t="str">
+        <v xml:space="preserve"> New exterior paint</v>
+      </c>
+      <c r="M4" t="str">
+        <v xml:space="preserve"> Good shape - needs updating"</v>
       </c>
     </row>
     <row r="5">
@@ -535,7 +547,7 @@
         <v>Not Found</v>
       </c>
       <c r="E5" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F5" t="str">
         <v>3</v>
@@ -547,7 +559,13 @@
         <v>1909</v>
       </c>
       <c r="I5" t="str">
-        <v>"Garage converted legally with permits to make it 4/3. Screened pool. Needs a new roof and updates"</v>
+        <v>"Garage converted legally to 4/3</v>
+      </c>
+      <c r="J5" t="str">
+        <v xml:space="preserve"> Screened pool</v>
+      </c>
+      <c r="K5" t="str">
+        <v xml:space="preserve"> Needs new roof and updates"</v>
       </c>
     </row>
     <row r="6">
@@ -564,7 +582,7 @@
         <v>Not Found</v>
       </c>
       <c r="E6" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F6" t="str">
         <v>2</v>
@@ -576,13 +594,19 @@
         <v>1624</v>
       </c>
       <c r="I6" t="str">
-        <v>"Needs interior rehab. Roof 5 years old</v>
+        <v>"Needs interior rehab</v>
       </c>
       <c r="J6" t="str">
-        <v xml:space="preserve"> central AC. 55 and older community. Buyer to assume tenant</v>
+        <v xml:space="preserve"> Roof 5 years old</v>
       </c>
       <c r="K6" t="str">
-        <v xml:space="preserve"> tenant leaving March"</v>
+        <v xml:space="preserve"> Central AC</v>
+      </c>
+      <c r="L6" t="str">
+        <v xml:space="preserve"> 55+ community</v>
+      </c>
+      <c r="M6" t="str">
+        <v xml:space="preserve"> Buyer to assume tenant leaving in March"</v>
       </c>
     </row>
     <row r="7">
@@ -599,7 +623,7 @@
         <v>Not Found</v>
       </c>
       <c r="E7" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F7" t="str">
         <v>3</v>
@@ -611,16 +635,34 @@
         <v>1249</v>
       </c>
       <c r="I7" t="str">
-        <v>"2 bedroom</v>
+        <v>"Carport</v>
       </c>
       <c r="J7" t="str">
-        <v xml:space="preserve"> 1 bathroom. Carport. Huge driveway. Roof 2022</v>
+        <v xml:space="preserve"> Huge driveway</v>
       </c>
       <c r="K7" t="str">
+        <v xml:space="preserve"> Roof 2022</v>
+      </c>
+      <c r="L7" t="str">
         <v xml:space="preserve"> AC 2016</v>
       </c>
-      <c r="L7" t="str">
-        <v xml:space="preserve"> water heater 2024. Detached workshop. Corner lot. Fenced in. Low DOM area. Only active in subdivision"</v>
+      <c r="M7" t="str">
+        <v xml:space="preserve"> Water heater 2024</v>
+      </c>
+      <c r="N7" t="str">
+        <v xml:space="preserve"> Detached workshop</v>
+      </c>
+      <c r="O7" t="str">
+        <v xml:space="preserve"> Corner lot</v>
+      </c>
+      <c r="P7" t="str">
+        <v xml:space="preserve"> Fenced in</v>
+      </c>
+      <c r="Q7" t="str">
+        <v xml:space="preserve"> Low DOM area</v>
+      </c>
+      <c r="R7" t="str">
+        <v xml:space="preserve"> Only active in subdivision"</v>
       </c>
     </row>
     <row r="8">
@@ -637,7 +679,7 @@
         <v>Not Found</v>
       </c>
       <c r="E8" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F8" t="str">
         <v>2</v>
@@ -649,7 +691,13 @@
         <v>888</v>
       </c>
       <c r="I8" t="str">
-        <v>"Garage. 55+ community. Needs some updates"</v>
+        <v>"Garage</v>
+      </c>
+      <c r="J8" t="str">
+        <v xml:space="preserve"> 55+ community</v>
+      </c>
+      <c r="K8" t="str">
+        <v xml:space="preserve"> Needs some updates"</v>
       </c>
     </row>
     <row r="9">
@@ -666,7 +714,7 @@
         <v>Not Found</v>
       </c>
       <c r="E9" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F9" t="str">
         <v>2</v>
@@ -678,7 +726,22 @@
         <v>950</v>
       </c>
       <c r="I9" t="str">
-        <v>"55+ community. All new appliances. Roof inspected with 6 years left. HVAC just replaced with new mini-split system. HOA $276 monthly. 2 year rental restriction"</v>
+        <v>"55+ community</v>
+      </c>
+      <c r="J9" t="str">
+        <v xml:space="preserve"> All new appliances</v>
+      </c>
+      <c r="K9" t="str">
+        <v xml:space="preserve"> Roof inspected with 6 years left</v>
+      </c>
+      <c r="L9" t="str">
+        <v xml:space="preserve"> New mini-split HVAC system</v>
+      </c>
+      <c r="M9" t="str">
+        <v xml:space="preserve"> HOA $276 monthly</v>
+      </c>
+      <c r="N9" t="str">
+        <v xml:space="preserve"> 2 year rental restriction"</v>
       </c>
     </row>
     <row r="10">
@@ -695,7 +758,7 @@
         <v>Not Found</v>
       </c>
       <c r="E10" t="str">
-        <v>"Single Family"</v>
+        <v>Single Family</v>
       </c>
       <c r="F10" t="str">
         <v>4</v>
@@ -707,7 +770,13 @@
         <v>1200</v>
       </c>
       <c r="I10" t="str">
-        <v>"Needs full rehab. On city water/sewer. Roof replaced 6 years ago. Roof leaks"</v>
+        <v>"Needs full rehab</v>
+      </c>
+      <c r="J10" t="str">
+        <v xml:space="preserve"> On city water/sewer</v>
+      </c>
+      <c r="K10" t="str">
+        <v xml:space="preserve"> Roof replaced 6 years ago but leaks"</v>
       </c>
     </row>
     <row r="11">
@@ -717,7 +786,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>